<commit_message>
Changes in Overview Diagram
</commit_message>
<xml_diff>
--- a/docs/images/overview.xlsx
+++ b/docs/images/overview.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reinhardt\firma\Hasenzagl\Magenta\working\oscake-documentation\docs\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0E2C25-FCE2-4B87-8386-19E9A8F2D270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CCCD05A-A434-4FF3-A71D-D3D81E7CD845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{74579933-400F-4051-B20C-7F9D550BA588}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>(curation directory; scan-results-)</t>
   </si>
   <si>
-    <t xml:space="preserve"> cache; source codes directory)</t>
-  </si>
-  <si>
     <r>
       <t>native-scan-results/</t>
     </r>
@@ -129,6 +126,9 @@
   </si>
   <si>
     <t>optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cache; source codes cache)</t>
   </si>
 </sst>
 </file>
@@ -219,6 +219,60 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>157370</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>49696</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>165653</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>57978</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="39" name="Gerade Verbindung mit Pfeil 38">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B934A5D5-08D0-431B-A183-C4A80044C1E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4961283" y="4174435"/>
+          <a:ext cx="728870" cy="8282"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:headEnd type="arrow" w="lg" len="lg"/>
+          <a:tailEnd type="arrow" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -1244,15 +1298,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>230533</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>230533</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>74267</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1267,8 +1321,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13938250" y="3867150"/>
-          <a:ext cx="0" cy="1003300"/>
+          <a:off x="4554055" y="4315239"/>
+          <a:ext cx="0" cy="885963"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1295,15 +1349,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>230533</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>93317</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
+      <xdr:colOff>230533</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:rowOff>93317</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1318,8 +1372,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13176250" y="4705350"/>
-          <a:ext cx="762000" cy="0"/>
+          <a:off x="4313859" y="5029752"/>
+          <a:ext cx="240196" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1348,15 +1402,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>236883</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>80617</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:colOff>236883</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:rowOff>80617</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1371,8 +1425,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="13182600" y="4876800"/>
-          <a:ext cx="762000" cy="0"/>
+          <a:off x="4320209" y="5207552"/>
+          <a:ext cx="240196" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1639,6 +1693,386 @@
           <a:avLst/>
         </a:prstGeom>
         <a:ln w="22225">
+          <a:tailEnd type="arrow" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>149087</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>66261</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>66260</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="44" name="Gruppieren 43">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3CE971A-1954-47A7-A440-F39FC53BE221}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5673587" y="3429000"/>
+          <a:ext cx="1118152" cy="571499"/>
+          <a:chOff x="5673587" y="3429000"/>
+          <a:chExt cx="1118152" cy="571499"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="23" name="Flussdiagramm: Magnetplattenspeicher 22">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F5E0765-2E3F-4612-8736-7572D9D3D87E}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5673588" y="3429000"/>
+            <a:ext cx="1101586" cy="513522"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDisk">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-AT" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="25" name="Textfeld 24">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB6ED313-FA18-486F-85F3-815990CD1189}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5673587" y="3544955"/>
+            <a:ext cx="1118152" cy="455544"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1100"/>
+              <a:t>Source-Codes Cache</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>149087</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>107674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>66261</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>115955</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="43" name="Gruppieren 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BC2A1D9-3BC6-4697-B7E2-B39AEFA959B2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="5673587" y="4041913"/>
+          <a:ext cx="1118152" cy="571499"/>
+          <a:chOff x="5673587" y="4041913"/>
+          <a:chExt cx="1118152" cy="571499"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="32" name="Flussdiagramm: Magnetplattenspeicher 31">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACBF6734-F683-440D-983A-1E9431D4993F}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5673588" y="4041913"/>
+            <a:ext cx="1101586" cy="513522"/>
+          </a:xfrm>
+          <a:prstGeom prst="flowChartMagneticDisk">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:lumMod val="40000"/>
+              <a:lumOff val="60000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="l"/>
+            <a:endParaRPr lang="de-AT" sz="1100"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+      <xdr:sp macro="" textlink="">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="34" name="Textfeld 33">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A98AF221-C7E2-4B0E-B364-544FDF1A2E70}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="5673587" y="4157868"/>
+            <a:ext cx="1118152" cy="455544"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:noFill/>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr"/>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1100"/>
+              <a:t>Scan-Results Cache</a:t>
+            </a:r>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>183597</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>90281</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>189947</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>77582</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="35" name="Gerade Verbindung mit Pfeil 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D775FA2C-11C2-416B-B42F-4FFA356D9472}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="8151467" y="3453020"/>
+          <a:ext cx="6350" cy="368301"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:headEnd type="arrow" w="lg" len="lg"/>
+          <a:tailEnd type="arrow" w="lg" len="lg"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>165652</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144941</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>140804</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>149084</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="36" name="Gerade Verbindung mit Pfeil 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11C91BC6-9EF1-4B4C-82B5-DE0AE7D86ACC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="4969565" y="3698180"/>
+          <a:ext cx="695739" cy="4143"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="22225">
+          <a:headEnd type="arrow" w="lg" len="lg"/>
           <a:tailEnd type="arrow" w="lg" len="lg"/>
         </a:ln>
       </xdr:spPr>
@@ -1962,7 +2396,7 @@
   <dimension ref="B1:W31"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2023,7 +2457,7 @@
         <v>10</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
@@ -2064,7 +2498,7 @@
     </row>
     <row r="22" spans="2:15" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C22" s="7" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="2:15" x14ac:dyDescent="0.25">
@@ -2105,10 +2539,10 @@
         <v>0</v>
       </c>
       <c r="N31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O31" t="s">
         <v>21</v>
-      </c>
-      <c r="O31" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Renmaing of Injector to MetaDataManager
</commit_message>
<xml_diff>
--- a/docs/images/overview.xlsx
+++ b/docs/images/overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\reinhardt\firma\Hasenzagl\Magenta\working\oscake-documentation\docs\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B6501A2-49A5-41BF-9A95-2C6FFFC4AF98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A826BCEB-B6E2-43FF-92E5-A408262BE237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="465" windowWidth="23520" windowHeight="14580" xr2:uid="{74579933-400F-4051-B20C-7F9D550BA588}"/>
+    <workbookView xWindow="2820" yWindow="2325" windowWidth="23520" windowHeight="12165" xr2:uid="{74579933-400F-4051-B20C-7F9D550BA588}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -195,16 +195,16 @@
     <t>[project]_selected.zip</t>
   </si>
   <si>
-    <t>OSCake-Report_injected.oscc</t>
-  </si>
-  <si>
-    <t>[project]_injected.zip</t>
-  </si>
-  <si>
     <t>1. als pdf exportieren</t>
   </si>
   <si>
     <t>2. pdf mit irfanView öffnen und als jpg speichern</t>
+  </si>
+  <si>
+    <t>OSCake-Report_metadata.oscc</t>
+  </si>
+  <si>
+    <t>[project]_metadata.zip</t>
   </si>
 </sst>
 </file>
@@ -4596,15 +4596,15 @@
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" tIns="72000" bIns="72000" rtlCol="0" anchor="ctr">
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" tIns="36000" bIns="36000" rtlCol="0" anchor="ctr">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr"/>
           <a:r>
-            <a:rPr lang="de-DE" sz="1600"/>
-            <a:t>Injector</a:t>
+            <a:rPr lang="de-DE" sz="1400"/>
+            <a:t>MetaData-Manager</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -5143,8 +5143,8 @@
   </sheetPr>
   <dimension ref="B1:AF61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AD41" sqref="AD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5157,12 +5157,12 @@
         <v>13</v>
       </c>
       <c r="AF1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="2:32" x14ac:dyDescent="0.25">
       <c r="AF2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:32" x14ac:dyDescent="0.25">
@@ -5396,12 +5396,12 @@
     </row>
     <row r="48" spans="3:17" x14ac:dyDescent="0.25">
       <c r="K48" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="49" spans="2:23" x14ac:dyDescent="0.25">
       <c r="K49" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="52" spans="2:23" ht="17.25" x14ac:dyDescent="0.25">

</xml_diff>